<commit_message>
Updates to push app before demo
</commit_message>
<xml_diff>
--- a/Clean_Data/CGAC_list.xlsx
+++ b/Clean_Data/CGAC_list.xlsx
@@ -481,7 +481,7 @@
     <t>Architect of the Capitol</t>
   </si>
   <si>
-    <t>Armed forces Retirement Home</t>
+    <t>Armed Forces Retirement Home</t>
   </si>
   <si>
     <t>Barry Goldwater Scholarship and Excellence In Education Fund</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">Council of the Inspectors General on Integrity and Efficiency </t>
   </si>
   <si>
-    <t>Court Services and offender Supervision Agency for the District of Columbia</t>
+    <t>Court Services and Offender Supervision Agency for the District of Columbia</t>
   </si>
   <si>
     <t>Defense Nuclear Facilities Safety Board</t>

</xml_diff>

<commit_message>
Further update to CGAC list
</commit_message>
<xml_diff>
--- a/Clean_Data/CGAC_list.xlsx
+++ b/Clean_Data/CGAC_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
   <si>
     <t>CGAC</t>
   </si>
@@ -28,87 +28,42 @@
     <t>302</t>
   </si>
   <si>
-    <t>306</t>
-  </si>
-  <si>
-    <t>530</t>
-  </si>
-  <si>
     <t>072</t>
   </si>
   <si>
-    <t>074</t>
-  </si>
-  <si>
     <t>309</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
     <t>084</t>
   </si>
   <si>
-    <t>313</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
     <t>514</t>
   </si>
   <si>
     <t>581</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>056</t>
-  </si>
-  <si>
     <t>510</t>
   </si>
   <si>
-    <t>465</t>
-  </si>
-  <si>
-    <t>582</t>
-  </si>
-  <si>
-    <t>323</t>
-  </si>
-  <si>
-    <t>326</t>
-  </si>
-  <si>
     <t>338</t>
   </si>
   <si>
     <t>339</t>
   </si>
   <si>
-    <t>008</t>
-  </si>
-  <si>
     <t>061</t>
   </si>
   <si>
     <t>485</t>
   </si>
   <si>
-    <t>580</t>
-  </si>
-  <si>
     <t>096</t>
   </si>
   <si>
     <t>542</t>
   </si>
   <si>
-    <t>511</t>
-  </si>
-  <si>
     <t>347</t>
   </si>
   <si>
@@ -145,9 +100,6 @@
     <t>015</t>
   </si>
   <si>
-    <t>016</t>
-  </si>
-  <si>
     <t>019</t>
   </si>
   <si>
@@ -172,48 +124,21 @@
     <t>525</t>
   </si>
   <si>
-    <t>531</t>
-  </si>
-  <si>
     <t>068</t>
   </si>
   <si>
     <t>045</t>
   </si>
   <si>
-    <t>011</t>
-  </si>
-  <si>
     <t>083</t>
   </si>
   <si>
-    <t>352</t>
-  </si>
-  <si>
-    <t>912</t>
-  </si>
-  <si>
     <t>027</t>
   </si>
   <si>
-    <t>051</t>
-  </si>
-  <si>
     <t>360</t>
   </si>
   <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>913</t>
-  </si>
-  <si>
-    <t>914</t>
-  </si>
-  <si>
-    <t>537</t>
-  </si>
-  <si>
     <t>054</t>
   </si>
   <si>
@@ -226,84 +151,30 @@
     <t>368</t>
   </si>
   <si>
-    <t>915</t>
-  </si>
-  <si>
-    <t>473</t>
-  </si>
-  <si>
-    <t>026</t>
-  </si>
-  <si>
     <t>029</t>
   </si>
   <si>
-    <t>920</t>
-  </si>
-  <si>
     <t>047</t>
   </si>
   <si>
     <t>005</t>
   </si>
   <si>
-    <t>004</t>
-  </si>
-  <si>
     <t>471</t>
   </si>
   <si>
-    <t>372</t>
-  </si>
-  <si>
-    <t>578</t>
-  </si>
-  <si>
-    <t>584</t>
-  </si>
-  <si>
-    <t>373</t>
-  </si>
-  <si>
     <t>474</t>
   </si>
   <si>
-    <t>467</t>
-  </si>
-  <si>
-    <t>376</t>
-  </si>
-  <si>
     <t>034</t>
   </si>
   <si>
-    <t>381</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>283</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
     <t>387</t>
   </si>
   <si>
-    <t>235</t>
-  </si>
-  <si>
     <t>389</t>
   </si>
   <si>
-    <t>479</t>
-  </si>
-  <si>
     <t>524</t>
   </si>
   <si>
@@ -319,9 +190,6 @@
     <t>394</t>
   </si>
   <si>
-    <t>413</t>
-  </si>
-  <si>
     <t>025</t>
   </si>
   <si>
@@ -331,87 +199,39 @@
     <t>418</t>
   </si>
   <si>
-    <t>538</t>
-  </si>
-  <si>
     <t>420</t>
   </si>
   <si>
     <t>421</t>
   </si>
   <si>
-    <t>575</t>
-  </si>
-  <si>
     <t>049</t>
   </si>
   <si>
     <t>424</t>
   </si>
   <si>
-    <t>082</t>
-  </si>
-  <si>
-    <t>573</t>
-  </si>
-  <si>
     <t>031</t>
   </si>
   <si>
     <t>432</t>
   </si>
   <si>
-    <t>434</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
     <t>024</t>
   </si>
   <si>
     <t>062</t>
   </si>
   <si>
-    <t>534</t>
-  </si>
-  <si>
     <t>431</t>
   </si>
   <si>
-    <t>377</t>
-  </si>
-  <si>
-    <t>310</t>
-  </si>
-  <si>
     <t>071</t>
   </si>
   <si>
-    <t>579</t>
-  </si>
-  <si>
-    <t>018</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>535</t>
-  </si>
-  <si>
-    <t>526</t>
-  </si>
-  <si>
     <t>060</t>
   </si>
   <si>
-    <t>539</t>
-  </si>
-  <si>
-    <t>576</t>
-  </si>
-  <si>
     <t>050</t>
   </si>
   <si>
@@ -421,129 +241,51 @@
     <t>073</t>
   </si>
   <si>
-    <t>033</t>
-  </si>
-  <si>
     <t>028</t>
   </si>
   <si>
-    <t>527</t>
-  </si>
-  <si>
-    <t>453</t>
-  </si>
-  <si>
     <t>472</t>
   </si>
   <si>
-    <t>455</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>023</t>
-  </si>
-  <si>
-    <t>476</t>
-  </si>
-  <si>
-    <t>486</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>458</t>
-  </si>
-  <si>
-    <t>519</t>
-  </si>
-  <si>
     <t>Administrative Conference of the U. S.</t>
   </si>
   <si>
-    <t>Advisory Council on Historic Preservation</t>
-  </si>
-  <si>
-    <t>Affordable Housing Program</t>
-  </si>
-  <si>
     <t>Agency for International Development</t>
   </si>
   <si>
-    <t>American Battle Monuments Commission</t>
-  </si>
-  <si>
     <t>Appalachian Regional Commission</t>
   </si>
   <si>
-    <t>Architect of the Capitol</t>
-  </si>
-  <si>
     <t>Armed Forces Retirement Home</t>
   </si>
   <si>
-    <t>Barry Goldwater Scholarship and Excellence In Education Fund</t>
-  </si>
-  <si>
-    <t>Botanic Garden</t>
-  </si>
-  <si>
     <t>Broadcasting Board of Governors</t>
   </si>
   <si>
     <t>Bureau of Consumer Financial Protection</t>
   </si>
   <si>
-    <t>Capitol Police</t>
-  </si>
-  <si>
-    <t>Central Intelligence Agency</t>
-  </si>
-  <si>
     <t>Chemical Safety and Hazard Investigation Board</t>
   </si>
   <si>
-    <t>Christopher Columbus Fellowship Foundation</t>
-  </si>
-  <si>
-    <t>Civilian Property Realignment Board</t>
-  </si>
-  <si>
-    <t>Commission of Fine Arts</t>
-  </si>
-  <si>
-    <t>Commission on Civil Rights</t>
-  </si>
-  <si>
     <t>Committee for Purchase From People Who Are Blind or Severely Disabled</t>
   </si>
   <si>
     <t>Commodity Futures Trading Commission</t>
   </si>
   <si>
-    <t>Congressional Budget Office</t>
-  </si>
-  <si>
     <t>Consumer Product Safety Commission</t>
   </si>
   <si>
     <t>Corporation for National and Community Service</t>
   </si>
   <si>
-    <t>Corporation for Travel Promotion</t>
-  </si>
-  <si>
     <t>Corps of Engineers - Civil Works</t>
   </si>
   <si>
     <t xml:space="preserve">Council of the Inspectors General on Integrity and Efficiency </t>
   </si>
   <si>
-    <t>Court Services and Offender Supervision Agency for the District of Columbia</t>
-  </si>
-  <si>
     <t>Defense Nuclear Facilities Safety Board</t>
   </si>
   <si>
@@ -580,9 +322,6 @@
     <t>Department of Justice</t>
   </si>
   <si>
-    <t>Department of Labor</t>
-  </si>
-  <si>
     <t>Department of State</t>
   </si>
   <si>
@@ -607,48 +346,21 @@
     <t>Election Assistance Commission</t>
   </si>
   <si>
-    <t>Electric Reliability Organization</t>
-  </si>
-  <si>
     <t>Environmental Protection Agency</t>
   </si>
   <si>
     <t>Equal Employment Opportunity Commission</t>
   </si>
   <si>
-    <t>Executive Office of the President</t>
-  </si>
-  <si>
     <t>Export-Import Bank of the U.S.</t>
   </si>
   <si>
-    <t>Farm Credit Administration</t>
-  </si>
-  <si>
-    <t>Farm Credit System</t>
-  </si>
-  <si>
     <t>Federal Communications Commission</t>
   </si>
   <si>
-    <t>Federal Deposit Insurance Corporation</t>
-  </si>
-  <si>
     <t>Federal Election Commission</t>
   </si>
   <si>
-    <t>Federal Financial Institutions Examination Council</t>
-  </si>
-  <si>
-    <t>Federal Home Loan Bank System</t>
-  </si>
-  <si>
-    <t>Federal Home Loan Mortgage Corporation</t>
-  </si>
-  <si>
-    <t>Federal Housing Finance Agency</t>
-  </si>
-  <si>
     <t>Federal Labor Relations Authority</t>
   </si>
   <si>
@@ -661,84 +373,30 @@
     <t>Federal Mine Safety and Health Review Commission</t>
   </si>
   <si>
-    <t>Federal National Mortgage Association</t>
-  </si>
-  <si>
-    <t>Federal Permitting Improvement Steering Council</t>
-  </si>
-  <si>
-    <t>Federal Retirement Thrift Investment Board</t>
-  </si>
-  <si>
     <t>Federal Trade Commission</t>
   </si>
   <si>
-    <t>Financing Vehicles and the Board of Governors of the Federal Reserve</t>
-  </si>
-  <si>
     <t>General Services Administration</t>
   </si>
   <si>
     <t>Government Accountability Office</t>
   </si>
   <si>
-    <t>Government Publishing Office</t>
-  </si>
-  <si>
     <t>Gulf Coast Ecosystem Restoration Council</t>
   </si>
   <si>
-    <t>Harry S Truman Scholarship Foundation</t>
-  </si>
-  <si>
-    <t>Independent Payment Advisory Board</t>
-  </si>
-  <si>
-    <t>Indian Law and order Commission</t>
-  </si>
-  <si>
-    <t>Institute of American Indian and Alaska Native Culture and Arts Development</t>
-  </si>
-  <si>
     <t>Institute of Museum Services and Library Services</t>
   </si>
   <si>
-    <t>Intelligence Community Management Account</t>
-  </si>
-  <si>
-    <t>Inter-Agency Council for Homeless</t>
-  </si>
-  <si>
     <t>International Trade Commission</t>
   </si>
   <si>
-    <t>James Madison Memorial Fellowship Foundation</t>
-  </si>
-  <si>
-    <t>Judicial Branch</t>
-  </si>
-  <si>
-    <t>Legislative Branch</t>
-  </si>
-  <si>
-    <t>Legislative Branch Boards and Commissions</t>
-  </si>
-  <si>
-    <t>Library of Congress</t>
-  </si>
-  <si>
     <t>Marine Mammal Commission</t>
   </si>
   <si>
-    <t xml:space="preserve">Medicare Payment Advisory Commission  </t>
-  </si>
-  <si>
     <t>Merit Systems Protection Board</t>
   </si>
   <si>
-    <t>Military Compensation and Retirement Modernization Commission</t>
-  </si>
-  <si>
     <t>Millenium Challenge Corporation</t>
   </si>
   <si>
@@ -754,9 +412,6 @@
     <t>National Capital Planning Commission</t>
   </si>
   <si>
-    <t>National Council on Disability</t>
-  </si>
-  <si>
     <t>National Credit Union Administration</t>
   </si>
   <si>
@@ -766,87 +421,39 @@
     <t>National Endowment for the Humanities</t>
   </si>
   <si>
-    <t>National Infrastructure Bank</t>
-  </si>
-  <si>
     <t>National Labor Relations Board</t>
   </si>
   <si>
     <t>National Mediation Board</t>
   </si>
   <si>
-    <t>National Railroad Passenger Corporation Office of the Inspector General</t>
-  </si>
-  <si>
     <t>National Science Foundation</t>
   </si>
   <si>
     <t>National Transportation Safety Board</t>
   </si>
   <si>
-    <t>Neighborhood Reinvestment Corporation</t>
-  </si>
-  <si>
-    <t>Northern Border Regional Commission</t>
-  </si>
-  <si>
     <t>Nuclear Regulatory Commission</t>
   </si>
   <si>
     <t>Occupational Safety and Health Review Commission</t>
   </si>
   <si>
-    <t>Office of Government Ethics</t>
-  </si>
-  <si>
-    <t>Office of Navajo and Hopi Indian Relocation</t>
-  </si>
-  <si>
     <t>Office of Personnel Management</t>
   </si>
   <si>
     <t>Office of Special Counsel</t>
   </si>
   <si>
-    <t>Office of the Federal Coordinator for Alaska Natural Gas Transportation Projects</t>
-  </si>
-  <si>
     <t>Office of the Nuclear Waste Negotiation</t>
   </si>
   <si>
-    <t>Other Commissions and Boards</t>
-  </si>
-  <si>
-    <t>Other Independent Agencies</t>
-  </si>
-  <si>
     <t>Overseas Private Investment Corporation</t>
   </si>
   <si>
-    <t>Patient-Centered Outcomes Research Trust Fund</t>
-  </si>
-  <si>
-    <t>Postal Service</t>
-  </si>
-  <si>
-    <t>Presidio Trust</t>
-  </si>
-  <si>
-    <t>Privacy and Civil Liberties Oversight Board</t>
-  </si>
-  <si>
-    <t>Public Company Accounting Oversight Board</t>
-  </si>
-  <si>
     <t>Railroad Retirement Board</t>
   </si>
   <si>
-    <t>Recovery Act Accountability and Transparency Board</t>
-  </si>
-  <si>
-    <t>Securities Investor Protection Corporation</t>
-  </si>
-  <si>
     <t>Securities and Exchange Commission</t>
   </si>
   <si>
@@ -856,43 +463,10 @@
     <t>Small Business Administration</t>
   </si>
   <si>
-    <t>Smithsonian Institution</t>
-  </si>
-  <si>
     <t>Social Security Administration</t>
   </si>
   <si>
-    <t>Standard Setting Body</t>
-  </si>
-  <si>
-    <t>State Justice Institute</t>
-  </si>
-  <si>
     <t>Surface Transportation Board</t>
-  </si>
-  <si>
-    <t>Tennessee Valley Authority</t>
-  </si>
-  <si>
-    <t>U.S. Court of Veteran Appeals</t>
-  </si>
-  <si>
-    <t>U.S. Tax Court</t>
-  </si>
-  <si>
-    <t>United Mine Workers of America Benefit Funds</t>
-  </si>
-  <si>
-    <t>United States Enrichment Corporation Fund</t>
-  </si>
-  <si>
-    <t>United States Holocaust Memorial Museum</t>
-  </si>
-  <si>
-    <t>United States Institute of Peace</t>
-  </si>
-  <si>
-    <t>Vietnam Education Foundation</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +824,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1277,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1285,7 +859,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1293,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1301,7 +875,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1309,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1317,7 +891,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1325,7 +899,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1333,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1341,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1349,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1357,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1365,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1373,7 +947,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1381,7 +955,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1389,7 +963,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1397,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1405,7 +979,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1413,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1421,7 +995,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1429,7 +1003,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1437,7 +1011,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1445,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>169</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1453,7 +1027,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1461,7 +1035,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1469,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1477,7 +1051,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1485,7 +1059,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1493,7 +1067,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1501,7 +1075,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1509,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1517,7 +1091,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1525,7 +1099,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1533,7 +1107,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1541,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1549,7 +1123,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1557,7 +1131,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1565,7 +1139,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1573,7 +1147,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1581,7 +1155,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1589,7 +1163,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1597,7 +1171,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1605,7 +1179,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1613,7 +1187,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1621,7 +1195,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1629,7 +1203,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1637,7 +1211,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1645,7 +1219,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1653,7 +1227,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1661,7 +1235,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1669,7 +1243,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1677,7 +1251,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1685,7 +1259,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1693,7 +1267,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1701,7 +1275,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1709,7 +1283,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1717,7 +1291,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1725,7 +1299,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1733,7 +1307,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1741,7 +1315,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1749,7 +1323,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1757,7 +1331,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1765,7 +1339,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1773,7 +1347,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1781,7 +1355,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1789,7 +1363,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1797,7 +1371,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1805,7 +1379,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1813,7 +1387,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1821,7 +1395,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1829,7 +1403,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1837,7 +1411,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1845,7 +1419,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1853,7 +1427,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1861,575 +1435,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>82</v>
-      </c>
-      <c r="B82" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>83</v>
-      </c>
-      <c r="B83" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>84</v>
-      </c>
-      <c r="B84" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>86</v>
-      </c>
-      <c r="B86" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>88</v>
-      </c>
-      <c r="B88" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>89</v>
-      </c>
-      <c r="B89" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>92</v>
-      </c>
-      <c r="B92" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>93</v>
-      </c>
-      <c r="B93" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>96</v>
-      </c>
-      <c r="B96" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
-        <v>97</v>
-      </c>
-      <c r="B97" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
-        <v>98</v>
-      </c>
-      <c r="B98" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
-        <v>99</v>
-      </c>
-      <c r="B99" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
-        <v>100</v>
-      </c>
-      <c r="B100" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
-        <v>101</v>
-      </c>
-      <c r="B101" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
-        <v>102</v>
-      </c>
-      <c r="B102" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
-        <v>103</v>
-      </c>
-      <c r="B103" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
-        <v>104</v>
-      </c>
-      <c r="B104" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
-        <v>105</v>
-      </c>
-      <c r="B105" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
-        <v>107</v>
-      </c>
-      <c r="B107" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
-        <v>108</v>
-      </c>
-      <c r="B108" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
-        <v>109</v>
-      </c>
-      <c r="B109" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
-        <v>110</v>
-      </c>
-      <c r="B110" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
-        <v>111</v>
-      </c>
-      <c r="B111" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
-        <v>112</v>
-      </c>
-      <c r="B112" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
-        <v>113</v>
-      </c>
-      <c r="B113" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
-        <v>115</v>
-      </c>
-      <c r="B115" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
-        <v>116</v>
-      </c>
-      <c r="B116" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
-        <v>117</v>
-      </c>
-      <c r="B117" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
-        <v>118</v>
-      </c>
-      <c r="B118" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" t="s">
-        <v>119</v>
-      </c>
-      <c r="B119" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
-        <v>120</v>
-      </c>
-      <c r="B120" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" t="s">
-        <v>121</v>
-      </c>
-      <c r="B121" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" t="s">
-        <v>122</v>
-      </c>
-      <c r="B122" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" t="s">
-        <v>123</v>
-      </c>
-      <c r="B123" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" t="s">
-        <v>124</v>
-      </c>
-      <c r="B124" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" t="s">
-        <v>125</v>
-      </c>
-      <c r="B125" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" t="s">
-        <v>126</v>
-      </c>
-      <c r="B126" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" t="s">
-        <v>127</v>
-      </c>
-      <c r="B127" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" t="s">
-        <v>128</v>
-      </c>
-      <c r="B128" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" t="s">
-        <v>129</v>
-      </c>
-      <c r="B129" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" t="s">
-        <v>130</v>
-      </c>
-      <c r="B130" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" t="s">
-        <v>131</v>
-      </c>
-      <c r="B131" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" t="s">
-        <v>132</v>
-      </c>
-      <c r="B132" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" t="s">
-        <v>133</v>
-      </c>
-      <c r="B133" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" t="s">
-        <v>134</v>
-      </c>
-      <c r="B134" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" t="s">
-        <v>135</v>
-      </c>
-      <c r="B135" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" t="s">
-        <v>136</v>
-      </c>
-      <c r="B136" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" t="s">
-        <v>137</v>
-      </c>
-      <c r="B137" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" t="s">
-        <v>138</v>
-      </c>
-      <c r="B138" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" t="s">
-        <v>139</v>
-      </c>
-      <c r="B139" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" t="s">
-        <v>140</v>
-      </c>
-      <c r="B140" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" t="s">
-        <v>141</v>
-      </c>
-      <c r="B141" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" t="s">
-        <v>142</v>
-      </c>
-      <c r="B142" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" t="s">
-        <v>143</v>
-      </c>
-      <c r="B143" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" t="s">
-        <v>144</v>
-      </c>
-      <c r="B144" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" t="s">
-        <v>145</v>
-      </c>
-      <c r="B145" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" t="s">
-        <v>146</v>
-      </c>
-      <c r="B146" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" t="s">
-        <v>147</v>
-      </c>
-      <c r="B147" t="s">
-        <v>292</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to CGAC list
</commit_message>
<xml_diff>
--- a/Clean_Data/CGAC_list.xlsx
+++ b/Clean_Data/CGAC_list.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alia/Documents/Github/SpendApp/Clean_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC83BDA8-B1A4-9E4F-801C-13E2B7A3E57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16680" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="411">
   <si>
     <t>CGAC</t>
   </si>
@@ -235,9 +241,6 @@
     <t>062</t>
   </si>
   <si>
-    <t>431</t>
-  </si>
-  <si>
     <t>071</t>
   </si>
   <si>
@@ -271,33 +274,15 @@
     <t>Armed Forces Retirement Home</t>
   </si>
   <si>
-    <t>Broadcasting Board of Governors</t>
-  </si>
-  <si>
     <t>Bureau of Consumer Financial Protection</t>
   </si>
   <si>
-    <t>Chemical Safety and Hazard Investigation Board</t>
-  </si>
-  <si>
-    <t>Committee for Purchase From People Who Are Blind or Severely Disabled</t>
-  </si>
-  <si>
     <t>Commodity Futures Trading Commission</t>
   </si>
   <si>
     <t>Consumer Product Safety Commission</t>
   </si>
   <si>
-    <t>Corporation for National and Community Service</t>
-  </si>
-  <si>
-    <t>Corps of Engineers - Civil Works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Council of the Inspectors General on Integrity and Efficiency </t>
-  </si>
-  <si>
     <t>Defense Nuclear Facilities Safety Board</t>
   </si>
   <si>
@@ -397,9 +382,6 @@
     <t>Gulf Coast Ecosystem Restoration Council</t>
   </si>
   <si>
-    <t>Institute of Museum Services and Library Services</t>
-  </si>
-  <si>
     <t>International Trade Commission</t>
   </si>
   <si>
@@ -409,9 +391,6 @@
     <t>Merit Systems Protection Board</t>
   </si>
   <si>
-    <t>Millenium Challenge Corporation</t>
-  </si>
-  <si>
     <t>Morris K. Udall and Stewart L. Udall Foundation</t>
   </si>
   <si>
@@ -457,9 +436,6 @@
     <t>Office of Special Counsel</t>
   </si>
   <si>
-    <t>Office of the Nuclear Waste Negotiation</t>
-  </si>
-  <si>
     <t>Overseas Private Investment Corporation</t>
   </si>
   <si>
@@ -491,9 +467,6 @@
   </si>
   <si>
     <t>Consumer Product Safety Commission (CPSC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corps of Engineers </t>
   </si>
   <si>
     <t>Department of Agriculture (USDA)</t>
@@ -1152,13 +1125,142 @@
   </si>
   <si>
     <t>https://www.stb.gov/</t>
+  </si>
+  <si>
+    <t>U.S. Agency for Global Media</t>
+  </si>
+  <si>
+    <t>Corps of Engineers</t>
+  </si>
+  <si>
+    <t>U.S. International Development Finance Corporation (DFC)</t>
+  </si>
+  <si>
+    <t>AbilityOne Commission</t>
+  </si>
+  <si>
+    <t>The U.S. Agency for Global Media, formerly known as the Broadcasting Board of Governors, broadcasts news and information about the United States and the world to audiences abroad.</t>
+  </si>
+  <si>
+    <t>https://www.usagm.gov/</t>
+  </si>
+  <si>
+    <t>/federal-agencies/u-s-agency-for-global-media</t>
+  </si>
+  <si>
+    <t>https://www.abilityone.gov/</t>
+  </si>
+  <si>
+    <t>The AbilityOne Commission, formerly known as Committee for Purchase From People Who Are Blind or Severely Disabled, creates job opportunities for people who are blind or have other significant disabilities in the manufacture and delivery of products and services to the Federal Government.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/u-s-abilityone-commission</t>
+  </si>
+  <si>
+    <t>U.S. Army Corps of Engineers</t>
+  </si>
+  <si>
+    <t>http://www.usace.army.mil/</t>
+  </si>
+  <si>
+    <t>The Army Corps of Engineers provides public engineering services in peace and war to strengthen national security, energize the economy, and reduce risks from disasters.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/u-s-army-corps-of-engineers</t>
+  </si>
+  <si>
+    <t>AmeriCorps</t>
+  </si>
+  <si>
+    <t>Formerly known as the Corporation for National and Community Service, AmeriCorps, and AmeriCorps Seniors engage volunteers in serving directly with nonprofit organizations to tackle the nation's most pressing challenges.</t>
+  </si>
+  <si>
+    <t>https://americorps.gov/</t>
+  </si>
+  <si>
+    <t>/federal-agencies/americorps</t>
+  </si>
+  <si>
+    <t>Council of the Inspectors General on Integrity and Efficiency</t>
+  </si>
+  <si>
+    <t>http://www.ignet.gov/</t>
+  </si>
+  <si>
+    <t>The Council of the Inspectors General on Integrity and Efficiency address integrity, economy, and effectiveness issues in the federal government.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/council-of-the-inspectors-general-on-integrity-and-efficiency</t>
+  </si>
+  <si>
+    <t>The U.S. International Development Finance Corporation (DFC) is America’s development bank. DFC partners with the private sector to finance solutions to the most critical challenges facing the developing world.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/u-s-international-development-finance-corporation</t>
+  </si>
+  <si>
+    <t>https://www.dfc.gov/</t>
+  </si>
+  <si>
+    <t>Chemical Safety Board</t>
+  </si>
+  <si>
+    <t>https://www.csb.gov/</t>
+  </si>
+  <si>
+    <t>The Chemical Safety Board investigates industrial chemical accidents.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/u-s-chemical-safety-board</t>
+  </si>
+  <si>
+    <t>https://oig.usaid.gov/OPIC</t>
+  </si>
+  <si>
+    <t>Established in 1971, the Overseas Private Investment Corporation (OPIC) serves as the U.S. Government’s development finance institution. It mobilizes private capital to help solve critical development challenges and in doing so, advances U.S. foreign policy.</t>
+  </si>
+  <si>
+    <t>https://www.mcc.gov/</t>
+  </si>
+  <si>
+    <t>Millennium Challenge Corporation</t>
+  </si>
+  <si>
+    <t>The Millennium Challenge Corporation partners with the best-governed poor countries worldwide to promote economic growth and help people lift themselves out of poverty.</t>
+  </si>
+  <si>
+    <t>/federal-agencies/millennium-challenge-corporation</t>
+  </si>
+  <si>
+    <t>https://www.restorethegulf.gov/</t>
+  </si>
+  <si>
+    <t>Institute of Museum and Library Services</t>
+  </si>
+  <si>
+    <t>/federal-agencies/institute-of-museum-and-library-services</t>
+  </si>
+  <si>
+    <t>The Institute of Museum and Library Services is a grant making organization that also conducts research and develops policy. The Institute helps libraries and museums innovate, fosters lifelong learning and cultural and civic engagement.</t>
+  </si>
+  <si>
+    <t>https://www.imls.gov/</t>
+  </si>
+  <si>
+    <t>Spurred by the Deepwater Horizon oil spill, the Resources and Ecosystems Sustainability, Tourist Opportunities, and Revived Economies of the Gulf Coast States Act (RESTORE Act) was signed into law by President Obama on July 6, 2012. The RESTORE Act calls for a regional approach to restoring the long-term health of the valuable natural ecosystem and economy of the Gulf Coast region. The RESTORE Act established the Gulf Coast Ecosystem Restoration Council (Council)</t>
+  </si>
+  <si>
+    <t>https://www.dccourts.gov/</t>
+  </si>
+  <si>
+    <t>The DC Courts are comprised of the DC Court of Appeals, the Superior Court of DC, and the Court System, which provides administrative support to both courts. The DC Courts are the third branch of the District of Columbia government. The Mayor presides over the executive branch and the Council of the District of Columbia is the legislative branch. The Courts hear and decide cases based on the evidence and the applicable law.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1221,12 +1323,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1234,6 +1337,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1280,7 +1391,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1312,9 +1423,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1346,6 +1475,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1521,14 +1668,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1556,1408 +1705,1532 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E5" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E6" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>368</v>
+      </c>
+      <c r="C7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D7" t="s">
+        <v>374</v>
+      </c>
+      <c r="E7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E8" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>393</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>393</v>
+      </c>
+      <c r="D9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E9" t="s">
+        <v>395</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="B10" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E10" t="s">
+        <v>376</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>382</v>
+      </c>
+      <c r="C13" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" t="s">
+        <v>383</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>378</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>369</v>
+      </c>
+      <c r="D14" t="s">
+        <v>381</v>
+      </c>
+      <c r="E14" t="s">
+        <v>380</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>386</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>386</v>
+      </c>
+      <c r="D15" t="s">
+        <v>389</v>
+      </c>
+      <c r="E15" t="s">
+        <v>388</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="E17" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E19" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="E20" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="E21" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E23" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E25" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E26" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E27" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="E28" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="E29" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E30" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="E31" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="E32" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>104</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="E33" t="s">
+        <v>390</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>105</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" t="s">
+        <v>410</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E35" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D36" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="E36" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D37" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="E37" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E38" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E39" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="E40" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E41" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="E42" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="E43" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E44" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="E45" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D46" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="E46" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E47" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>119</v>
+      </c>
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s">
+        <v>408</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>404</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>404</v>
+      </c>
+      <c r="D49" t="s">
+        <v>405</v>
+      </c>
+      <c r="E49" t="s">
+        <v>406</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="E50" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="E51" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="E52" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>400</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="D53" t="s">
+        <v>402</v>
+      </c>
+      <c r="E53" t="s">
+        <v>401</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D54" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E54" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="E55" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="E56" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="E57" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D58" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="E58" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C59" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="E59" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C61" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="E61" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D62" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="E62" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E63" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E64" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C65" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E65" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E66" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D67" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E67" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E68" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>138</v>
+      </c>
+      <c r="C69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" t="s">
+        <v>398</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>139</v>
+      </c>
+      <c r="C70" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" t="s">
+        <v>240</v>
+      </c>
+      <c r="E70" t="s">
+        <v>301</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D71" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E71" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C72" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="E72" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D73" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E73" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D74" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E74" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="D75" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E75" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76" t="s">
-        <v>154</v>
-      </c>
-      <c r="C76" t="s">
-        <v>154</v>
-      </c>
-      <c r="D76" t="s">
-        <v>256</v>
-      </c>
-      <c r="E76" t="s">
-        <v>317</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6"/>
-    <hyperlink ref="F12" r:id="rId7"/>
-    <hyperlink ref="F16" r:id="rId8"/>
-    <hyperlink ref="F17" r:id="rId9"/>
-    <hyperlink ref="F18" r:id="rId10"/>
-    <hyperlink ref="F19" r:id="rId11"/>
-    <hyperlink ref="F20" r:id="rId12"/>
-    <hyperlink ref="F21" r:id="rId13"/>
-    <hyperlink ref="F22" r:id="rId14"/>
-    <hyperlink ref="F23" r:id="rId15"/>
-    <hyperlink ref="F24" r:id="rId16"/>
-    <hyperlink ref="F25" r:id="rId17"/>
-    <hyperlink ref="F26" r:id="rId18"/>
-    <hyperlink ref="F27" r:id="rId19"/>
-    <hyperlink ref="F28" r:id="rId20"/>
-    <hyperlink ref="F29" r:id="rId21"/>
-    <hyperlink ref="F30" r:id="rId22"/>
-    <hyperlink ref="F31" r:id="rId23"/>
-    <hyperlink ref="F32" r:id="rId24"/>
-    <hyperlink ref="F35" r:id="rId25"/>
-    <hyperlink ref="F36" r:id="rId26"/>
-    <hyperlink ref="F37" r:id="rId27"/>
-    <hyperlink ref="F38" r:id="rId28"/>
-    <hyperlink ref="F39" r:id="rId29"/>
-    <hyperlink ref="F40" r:id="rId30"/>
-    <hyperlink ref="F41" r:id="rId31"/>
-    <hyperlink ref="F42" r:id="rId32"/>
-    <hyperlink ref="F43" r:id="rId33"/>
-    <hyperlink ref="F44" r:id="rId34"/>
-    <hyperlink ref="F45" r:id="rId35"/>
-    <hyperlink ref="F46" r:id="rId36"/>
-    <hyperlink ref="F47" r:id="rId37"/>
-    <hyperlink ref="F50" r:id="rId38"/>
-    <hyperlink ref="F51" r:id="rId39"/>
-    <hyperlink ref="F52" r:id="rId40"/>
-    <hyperlink ref="F54" r:id="rId41"/>
-    <hyperlink ref="F55" r:id="rId42"/>
-    <hyperlink ref="F56" r:id="rId43"/>
-    <hyperlink ref="F57" r:id="rId44"/>
-    <hyperlink ref="F58" r:id="rId45"/>
-    <hyperlink ref="F59" r:id="rId46"/>
-    <hyperlink ref="F60" r:id="rId47"/>
-    <hyperlink ref="F61" r:id="rId48"/>
-    <hyperlink ref="F62" r:id="rId49"/>
-    <hyperlink ref="F63" r:id="rId50"/>
-    <hyperlink ref="F64" r:id="rId51"/>
-    <hyperlink ref="F65" r:id="rId52"/>
-    <hyperlink ref="F66" r:id="rId53"/>
-    <hyperlink ref="F67" r:id="rId54"/>
-    <hyperlink ref="F68" r:id="rId55"/>
-    <hyperlink ref="F71" r:id="rId56"/>
-    <hyperlink ref="F72" r:id="rId57"/>
-    <hyperlink ref="F73" r:id="rId58"/>
-    <hyperlink ref="F74" r:id="rId59"/>
-    <hyperlink ref="F75" r:id="rId60"/>
-    <hyperlink ref="F76" r:id="rId61"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F36" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F38" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F39" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F40" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F41" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F42" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F43" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F44" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F45" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F46" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F47" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F51" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F52" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F54" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F55" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F56" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F57" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F58" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F59" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F60" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F61" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F62" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F63" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F64" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F65" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F66" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F67" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F68" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F70" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F71" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F72" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F73" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F74" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F75" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F7" r:id="rId62" xr:uid="{603E26B4-8F4D-BD4E-BA17-FF70A02176CF}"/>
+    <hyperlink ref="F10" r:id="rId63" xr:uid="{DAB1550E-5534-104D-A68E-701E0C815314}"/>
+    <hyperlink ref="F14" r:id="rId64" xr:uid="{553ADB28-D47E-2A4A-A2AF-6068AE2615FA}"/>
+    <hyperlink ref="F13" r:id="rId65" xr:uid="{F1A8E586-564B-3A49-A41E-391DFDE8FE6D}"/>
+    <hyperlink ref="F15" r:id="rId66" xr:uid="{5D8B3FF9-0E48-5A48-981E-C7E2B630BDC4}"/>
+    <hyperlink ref="F33" r:id="rId67" xr:uid="{1A7B50E0-5D67-6A4C-AF2E-3549A6F41D9A}"/>
+    <hyperlink ref="F9" r:id="rId68" xr:uid="{ABFDE6C0-13E8-DB45-89B1-CCDFC24EC8D5}"/>
+    <hyperlink ref="F69" r:id="rId69" xr:uid="{3A3BC0DA-9140-7341-9A8E-21549E2738FD}"/>
+    <hyperlink ref="F53" r:id="rId70" xr:uid="{32017068-7D4C-074E-9EDC-07B5200CF40A}"/>
+    <hyperlink ref="F49" r:id="rId71" xr:uid="{19F3F839-05AF-294E-A32C-04981D4F22F2}"/>
+    <hyperlink ref="F48" r:id="rId72" xr:uid="{98DDA6C2-DFF4-9B42-889F-27CFFCBF0FF9}"/>
+    <hyperlink ref="F34" r:id="rId73" xr:uid="{F51523AB-9F26-F44F-BC3D-22FAD6C657F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>